<commit_message>
Many fixes and features around import and logging.
Now with import option to only import data that were updated in theire source file. Fixes around XLS-Import bug were we observed strange popups. Other smal imrovements of the logging ...
</commit_message>
<xml_diff>
--- a/LOCAL_SOURCES/SRC_EX2.xlsx
+++ b/LOCAL_SOURCES/SRC_EX2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\DEV\GIT\010_AntAI\LOCAL_SOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD722FD-4717-41C6-9063-F8A0CB4ED70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD6E8AA-DCAE-4A42-A92F-08AA8987D4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{32554E90-0A00-4DDA-ADEB-290997543BC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{32554E90-0A00-4DDA-ADEB-290997543BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="SRC_EXAMPLE_SCRIPTS" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SRC_EXAMPLE_SCRIPTS!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -221,91 +221,91 @@
     <t>Tim</t>
   </si>
   <si>
-    <t>Fin</t>
+    <t>20.2.2002</t>
+  </si>
+  <si>
+    <t>2.2.1988</t>
+  </si>
+  <si>
+    <t>1.1.1981</t>
+  </si>
+  <si>
+    <t>2.3.1981</t>
+  </si>
+  <si>
+    <t>1.5.1955</t>
+  </si>
+  <si>
+    <t>6.7.2022</t>
+  </si>
+  <si>
+    <t>3.2.1933</t>
+  </si>
+  <si>
+    <t>1.2.2005</t>
+  </si>
+  <si>
+    <t>Example Birthdaylist. You could add more info in the info_html or info_column in order to have something like a fried database or a customer database</t>
+  </si>
+  <si>
+    <t>chatbot_chatcpg_openai</t>
+  </si>
+  <si>
+    <t>chatcpg</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>CHATBOT</t>
+  </si>
+  <si>
+    <t>OpenAI Chatbot</t>
+  </si>
+  <si>
+    <t>https://chat.openai.com/chat</t>
+  </si>
+  <si>
+    <t>CMC</t>
+  </si>
+  <si>
+    <t>PATH</t>
+  </si>
+  <si>
+    <t>\\energy.local\MyCompany\Storing\MFC\PC_CAO_WATER\MFC_P\CMC\</t>
+  </si>
+  <si>
+    <t>CMK Unterlagen nach Monat in Subordnern organisiert</t>
+  </si>
+  <si>
+    <t>CMK</t>
+  </si>
+  <si>
+    <t>CMK_PATH_PFAD</t>
+  </si>
+  <si>
+    <t>google_searchengine</t>
+  </si>
+  <si>
+    <t>%goog%</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
+  </si>
+  <si>
+    <t>www.google.de</t>
+  </si>
+  <si>
+    <t>Finx</t>
   </si>
   <si>
     <t>Ted</t>
   </si>
   <si>
-    <t>20.2.2002</t>
-  </si>
-  <si>
-    <t>2.2.1988</t>
-  </si>
-  <si>
-    <t>1.1.1981</t>
-  </si>
-  <si>
-    <t>2.3.1981</t>
-  </si>
-  <si>
-    <t>1.5.1955</t>
-  </si>
-  <si>
-    <t>6.7.2022</t>
-  </si>
-  <si>
-    <t>3.2.1933</t>
-  </si>
-  <si>
-    <t>1.2.2005</t>
-  </si>
-  <si>
-    <t>Example Birthdaylist. You could add more info in the info_html or info_column in order to have something like a fried database or a customer database</t>
-  </si>
-  <si>
-    <t>chatbot_chatcpg_openai</t>
-  </si>
-  <si>
-    <t>chatcpg</t>
-  </si>
-  <si>
-    <t>LOCATION</t>
-  </si>
-  <si>
-    <t>WEB</t>
-  </si>
-  <si>
-    <t>CHATBOT</t>
-  </si>
-  <si>
-    <t>OpenAI Chatbot</t>
-  </si>
-  <si>
-    <t>https://chat.openai.com/chat</t>
-  </si>
-  <si>
-    <t>CMC</t>
-  </si>
-  <si>
-    <t>PATH</t>
-  </si>
-  <si>
-    <t>\\energy.local\MyCompany\Storing\MFC\PC_CAO_WATER\MFC_P\CMC\</t>
-  </si>
-  <si>
-    <t>CMK Unterlagen nach Monat in Subordnern organisiert</t>
-  </si>
-  <si>
-    <t>CMK</t>
-  </si>
-  <si>
-    <t>CMK_PATH_PFAD</t>
-  </si>
-  <si>
-    <t>google_searchengine</t>
-  </si>
-  <si>
-    <t>%goog%</t>
-  </si>
-  <si>
-    <t>SEARCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard google search </t>
-  </si>
-  <si>
-    <t>www.google.de</t>
+    <t>Standard google search.</t>
   </si>
 </sst>
 </file>
@@ -690,8 +690,8 @@
   <sheetPr codeName="Tabelle11"/>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,71 +736,71 @@
     </row>
     <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
         <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF9D830-78A5-4879-B6EC-0C71E2C895B6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,13 +1112,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1127,13 +1127,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1142,13 +1142,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -1157,13 +1157,13 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -1172,13 +1172,13 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1187,13 +1187,13 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,13 +1201,13 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,13 +1215,13 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1230,21 +1230,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE722083F2A25D4392EE06058483FC0B" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d2635c84cf28abf109e4a63ad270ea0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3f4c8009-b4bb-4066-a620-04dd32484973" xmlns:ns4="10da5715-5bdb-48d7-b4ac-ac79d3961ccf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6963a590176d61c364fc6c71a9790032" ns3:_="" ns4:_="">
     <xsd:import namespace="3f4c8009-b4bb-4066-a620-04dd32484973"/>
@@ -1415,10 +1400,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406E50AD-0C1B-46F9-8ACE-C6D020C96D6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95FDAC06-07B0-4D96-AD7F-E2449B9C7B61}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3f4c8009-b4bb-4066-a620-04dd32484973"/>
+    <ds:schemaRef ds:uri="10da5715-5bdb-48d7-b4ac-ac79d3961ccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1441,20 +1452,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95FDAC06-07B0-4D96-AD7F-E2449B9C7B61}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406E50AD-0C1B-46F9-8ACE-C6D020C96D6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3f4c8009-b4bb-4066-a620-04dd32484973"/>
-    <ds:schemaRef ds:uri="10da5715-5bdb-48d7-b4ac-ac79d3961ccf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>